<commit_message>
Changed time display in array to seconds
</commit_message>
<xml_diff>
--- a/MATLAB/Figures/Measurement/V8/Shelving-Sequences_Specs.xlsx
+++ b/MATLAB/Figures/Measurement/V8/Shelving-Sequences_Specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Desktop\Repositories\Barium_Shelving-Adiabatic-Passage\MATLAB\Figures\Measurement\V8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3935F5B3-B21B-4260-96C3-3C0C436FC890}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587BBE58-6F32-4464-A3CB-357E01198751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1044" yWindow="-96" windowWidth="22092" windowHeight="13152" xr2:uid="{184DAEC4-8724-4D26-99CF-40577115B37E}"/>
+    <workbookView xWindow="1044" yWindow="-96" windowWidth="22092" windowHeight="13152" activeTab="2" xr2:uid="{184DAEC4-8724-4D26-99CF-40577115B37E}"/>
   </bookViews>
   <sheets>
     <sheet name="7-Level" sheetId="8" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="89">
   <si>
     <t>Column1</t>
   </si>
@@ -89,30 +89,6 @@
     <t>Column8</t>
   </si>
   <si>
-    <t>1.2821455999707</t>
-  </si>
-  <si>
-    <t>1.3181030298265</t>
-  </si>
-  <si>
-    <t>1.3090202209188</t>
-  </si>
-  <si>
-    <t>1.3272488609979</t>
-  </si>
-  <si>
-    <t>1.2733105671904</t>
-  </si>
-  <si>
-    <t>2.2603911202811</t>
-  </si>
-  <si>
-    <t>2.1093738732015</t>
-  </si>
-  <si>
-    <t>1.8117050564914</t>
-  </si>
-  <si>
     <t>Step</t>
   </si>
   <si>
@@ -219,9 +195,6 @@
   </si>
   <si>
     <t>4103945765.16</t>
-  </si>
-  <si>
-    <t>1.3</t>
   </si>
   <si>
     <t>0.9988322949634</t>
@@ -934,7 +907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7ACD215-AF42-4B41-941C-7E6ED12B4E69}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -978,28 +951,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1007,25 +980,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>11</v>
+        <v>36</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.3272488609979E-3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1033,25 +1006,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>12</v>
+        <v>55</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.2733105671904001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1059,25 +1032,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.3272488609979E-3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1085,25 +1058,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1111,25 +1084,25 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1137,25 +1110,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1.2999999999999999E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1163,25 +1136,25 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1189,25 +1162,25 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>13</v>
+        <v>64</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2.2603911202810998E-3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1215,25 +1188,25 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1241,25 +1214,25 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>14</v>
+        <v>69</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2.1093738732015001E-3</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1267,25 +1240,25 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1293,25 +1266,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>11</v>
+        <v>36</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1.3272488609979E-3</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1319,25 +1292,25 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1345,25 +1318,25 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>12</v>
+        <v>55</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1.2733105671904001E-3</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1371,25 +1344,25 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1397,25 +1370,25 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1.3090202209187999E-3</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1423,25 +1396,25 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1449,25 +1422,25 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>15</v>
+        <v>64</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1.8117050564913999E-3</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1475,25 +1448,25 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1501,25 +1474,25 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>8</v>
+        <v>43</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1.2821455999707E-3</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1527,42 +1500,42 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1570,13 +1543,13 @@
         <v>0</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F26" s="5">
         <v>0</v>
@@ -1587,13 +1560,13 @@
         <v>1</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="F27" s="5">
         <v>0</v>
@@ -1604,13 +1577,13 @@
         <v>2</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F28" s="5">
         <v>0</v>
@@ -1621,10 +1594,10 @@
         <v>3</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5">
@@ -1644,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01FA352F-6AFF-43CD-9A43-30E5B46DF47C}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F17" sqref="B17:F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1688,28 +1661,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1717,25 +1690,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.3181030298264999E-3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1743,25 +1716,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.3090202209187999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1769,25 +1742,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1795,25 +1768,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.2999999999999999E-3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1821,25 +1794,25 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.3090202209187999E-3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1847,25 +1820,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1873,25 +1846,25 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1.3090202209187999E-3</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1899,25 +1872,25 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1925,25 +1898,25 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.3090202209187999E-3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1951,25 +1924,25 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1977,25 +1950,25 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1.3090202209187999E-3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2003,42 +1976,42 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.55000000000000004">
@@ -2046,13 +2019,13 @@
         <v>0</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F18" s="5">
         <v>0</v>
@@ -2063,13 +2036,13 @@
         <v>1</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="F19" s="5">
         <v>0</v>
@@ -2080,13 +2053,13 @@
         <v>2</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F20" s="5">
         <v>0</v>
@@ -2097,10 +2070,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5">
@@ -2120,8 +2093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0277561-7EE0-4C2E-94B3-85E4C94A3B2A}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2164,28 +2137,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2193,25 +2166,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.2821455999707E-3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2219,25 +2192,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>9</v>
+        <v>26</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.3181030298264999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2245,25 +2218,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2271,25 +2244,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1.2821455999707E-3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2297,42 +2270,42 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="6" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -2340,13 +2313,13 @@
         <v>0</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F11" s="5">
         <v>0</v>
@@ -2357,13 +2330,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="F12" s="5">
         <v>0</v>
@@ -2374,13 +2347,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F13" s="5">
         <v>0</v>
@@ -2391,10 +2364,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5">

</xml_diff>

<commit_message>
Improved 7-level sequence figure, changed scattering rate fluorescence
Added the respective colors to the 7-level sequence figures for paper.
Changed scattering rate for fluorescence measurement step to be 125MHz*1/3*0.756 ~30MHz, instead of 5MHz.
Moved error sources code to measurement folder
</commit_message>
<xml_diff>
--- a/MATLAB/Figures/Measurement/V8/Shelving-Sequences_Specs.xlsx
+++ b/MATLAB/Figures/Measurement/V8/Shelving-Sequences_Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brend\Desktop\Repositories\Barium_Shelving-Adiabatic-Passage\MATLAB\Figures\Measurement\V8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587BBE58-6F32-4464-A3CB-357E01198751}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98139FD5-051D-4CB0-8677-5B56245C0CC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1044" yWindow="-96" windowWidth="22092" windowHeight="13152" activeTab="2" xr2:uid="{184DAEC4-8724-4D26-99CF-40577115B37E}"/>
   </bookViews>
@@ -18,9 +18,9 @@
     <sheet name="3-Level" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="2" hidden="1">'3-Level'!$A$1:$H$7</definedName>
-    <definedName name="ExternalData_2" localSheetId="1" hidden="1">'5-Level'!$A$1:$H$14</definedName>
-    <definedName name="ExternalData_3" localSheetId="0" hidden="1">'7-Level'!$A$1:$H$23</definedName>
+    <definedName name="ExternalData_1" localSheetId="2" hidden="1">'3-Level'!$A$1:$I$7</definedName>
+    <definedName name="ExternalData_2" localSheetId="1" hidden="1">'5-Level'!$A$1:$I$14</definedName>
+    <definedName name="ExternalData_3" localSheetId="0" hidden="1">'7-Level'!$A$1:$I$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="112">
   <si>
     <t>Column1</t>
   </si>
@@ -119,33 +119,9 @@
     <t>0.99884260753763</t>
   </si>
   <si>
-    <t>31300</t>
-  </si>
-  <si>
-    <t>1013925407.5588</t>
-  </si>
-  <si>
-    <t>4109719937.11</t>
-  </si>
-  <si>
-    <t>4112319937.11</t>
-  </si>
-  <si>
     <t>0.99882794762124</t>
   </si>
   <si>
-    <t>30800</t>
-  </si>
-  <si>
-    <t>986265846.13128</t>
-  </si>
-  <si>
-    <t>4014850785.6</t>
-  </si>
-  <si>
-    <t>4017450785.6</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -164,18 +140,6 @@
     <t>0.99882971046946</t>
   </si>
   <si>
-    <t>30900</t>
-  </si>
-  <si>
-    <t>993109181.37498</t>
-  </si>
-  <si>
-    <t>3980750647.5</t>
-  </si>
-  <si>
-    <t>3983350647.5</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -185,18 +149,6 @@
     <t>0.99883564341252</t>
   </si>
   <si>
-    <t>31100</t>
-  </si>
-  <si>
-    <t>1000000000</t>
-  </si>
-  <si>
-    <t>4101345765.16</t>
-  </si>
-  <si>
-    <t>4103945765.16</t>
-  </si>
-  <si>
     <t>0.9988322949634</t>
   </si>
   <si>
@@ -212,27 +164,9 @@
     <t>0.99882040542544</t>
   </si>
   <si>
-    <t>30700</t>
-  </si>
-  <si>
-    <t>979469667.06954</t>
-  </si>
-  <si>
     <t>0.99884771116373</t>
   </si>
   <si>
-    <t>31400</t>
-  </si>
-  <si>
-    <t>1020960662.306</t>
-  </si>
-  <si>
-    <t>3998021567.7</t>
-  </si>
-  <si>
-    <t>4000621567.7</t>
-  </si>
-  <si>
     <t>0.99881959919827</t>
   </si>
   <si>
@@ -248,33 +182,9 @@
     <t>0.99839081139349</t>
   </si>
   <si>
-    <t>23100</t>
-  </si>
-  <si>
-    <t>575121707.18416</t>
-  </si>
-  <si>
-    <t>4105613074.98</t>
-  </si>
-  <si>
-    <t>4108213074.98</t>
-  </si>
-  <si>
     <t>0.99846491248735</t>
   </si>
   <si>
-    <t>24000</t>
-  </si>
-  <si>
-    <t>616296625.51329</t>
-  </si>
-  <si>
-    <t>4113587145.51</t>
-  </si>
-  <si>
-    <t>4116187145.51</t>
-  </si>
-  <si>
     <t>0.99882054956258</t>
   </si>
   <si>
@@ -287,12 +197,6 @@
     <t>0.99858763254548</t>
   </si>
   <si>
-    <t>26000</t>
-  </si>
-  <si>
-    <t>717556091.89369</t>
-  </si>
-  <si>
     <t>0.99884519595553</t>
   </si>
   <si>
@@ -308,18 +212,9 @@
     <t>Fluoresce</t>
   </si>
   <si>
-    <t>1762nm</t>
-  </si>
-  <si>
-    <t>Microwave</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
-    <t>Cooling</t>
-  </si>
-  <si>
     <t>TransferID</t>
   </si>
   <si>
@@ -330,13 +225,187 @@
   </si>
   <si>
     <t>Phase</t>
+  </si>
+  <si>
+    <t>Column52</t>
+  </si>
+  <si>
+    <t>FreqTrans</t>
+  </si>
+  <si>
+    <t>OmegaHide1</t>
+  </si>
+  <si>
+    <t>Pi/OmegaHide1</t>
+  </si>
+  <si>
+    <t>OmegaShelve1</t>
+  </si>
+  <si>
+    <t>AlphaShelve1</t>
+  </si>
+  <si>
+    <t>FreqTrans + Delta</t>
+  </si>
+  <si>
+    <t>FreqTrans - Delta</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>OmegaShelve2</t>
+  </si>
+  <si>
+    <t>OmegaShelve3</t>
+  </si>
+  <si>
+    <t>OmegaShelve4</t>
+  </si>
+  <si>
+    <t>OmegaShelve5</t>
+  </si>
+  <si>
+    <t>OmegaShelve6</t>
+  </si>
+  <si>
+    <t>OmegaShelve7</t>
+  </si>
+  <si>
+    <t>AlphaShelve2</t>
+  </si>
+  <si>
+    <t>AlphaShelve3</t>
+  </si>
+  <si>
+    <t>AlphaShelve4</t>
+  </si>
+  <si>
+    <t>AlphaShelve5</t>
+  </si>
+  <si>
+    <t>AlphaShelve6</t>
+  </si>
+  <si>
+    <t>AlphaShelve7</t>
+  </si>
+  <si>
+    <t>2*Delta/AlphaShelve1</t>
+  </si>
+  <si>
+    <t>1762nm (EOM)</t>
+  </si>
+  <si>
+    <t>Microwave (Horn)</t>
+  </si>
+  <si>
+    <t>RabiShelve1</t>
+  </si>
+  <si>
+    <t>RabiShelve2</t>
+  </si>
+  <si>
+    <t>RabiShelve3</t>
+  </si>
+  <si>
+    <t>RabiShelve4</t>
+  </si>
+  <si>
+    <t>RabiShelve5</t>
+  </si>
+  <si>
+    <t>RabiShelve6</t>
+  </si>
+  <si>
+    <t>RabiShelve7</t>
+  </si>
+  <si>
+    <t>RabiShelve8</t>
+  </si>
+  <si>
+    <t>RabiShelve9</t>
+  </si>
+  <si>
+    <t>RabiShelve10</t>
+  </si>
+  <si>
+    <t>RabiShelve11</t>
+  </si>
+  <si>
+    <t>AlphaShelve8</t>
+  </si>
+  <si>
+    <t>AlphaShelve9</t>
+  </si>
+  <si>
+    <t>AlphaShelve10</t>
+  </si>
+  <si>
+    <t>AlphaShelve11</t>
+  </si>
+  <si>
+    <t>2*Delta/AlphaShelve2</t>
+  </si>
+  <si>
+    <t>2*Delta/AlphaShelve3</t>
+  </si>
+  <si>
+    <t>2*Delta/AlphaShelve4</t>
+  </si>
+  <si>
+    <t>2*Delta/AlphaShelve5</t>
+  </si>
+  <si>
+    <t>2*Delta/AlphaShelve6</t>
+  </si>
+  <si>
+    <t>2*Delta/AlphaShelve7</t>
+  </si>
+  <si>
+    <t>2*Delta/AlphaShelve8</t>
+  </si>
+  <si>
+    <t>2*Delta/AlphaShelve9</t>
+  </si>
+  <si>
+    <t>2*Delta/AlphaShelve10</t>
+  </si>
+  <si>
+    <t>2*Delta/AlphaShelve11</t>
+  </si>
+  <si>
+    <t>OmegaHide2</t>
+  </si>
+  <si>
+    <t>OmegaHide3</t>
+  </si>
+  <si>
+    <t>OmegaHide4</t>
+  </si>
+  <si>
+    <t>Pi/OmegaHide2</t>
+  </si>
+  <si>
+    <t>Pi/OmegaHide3</t>
+  </si>
+  <si>
+    <t>Pi/OmegaHide4</t>
+  </si>
+  <si>
+    <t>Omegashelve3</t>
+  </si>
+  <si>
+    <t>1762nm(EOM)</t>
+  </si>
+  <si>
+    <t>Cooling Lasers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,8 +419,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,6 +454,24 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+        <bgColor rgb="FF70AD47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FFE2EFDA"/>
       </patternFill>
     </fill>
   </fills>
@@ -377,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -395,41 +505,37 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="27">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -492,6 +598,45 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -506,15 +651,281 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>96520</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>33266</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>134284</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F251CDC4-9C12-4F91-ADBA-4A9C2DB83BF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9057640" y="4221480"/>
+          <a:ext cx="6667746" cy="7982884"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>147320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>198178</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>88658</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{195C479C-757D-426A-BB04-1C0C092712CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15935960" y="5085080"/>
+          <a:ext cx="6995218" cy="3416058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>198178</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>151816</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1C0D6C1-174D-4B55-87BE-1ECC09EC0ADF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15935960" y="8823960"/>
+          <a:ext cx="6995218" cy="3397936"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>110490</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>121672</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{944375F5-22AF-49C7-8E60-ECD33E725634}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9513570" y="2670810"/>
+          <a:ext cx="10058400" cy="6960622"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>521970</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>31388</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57F80C97-434F-4ADD-93BD-3AC6626A9D85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9521190" y="1276350"/>
+          <a:ext cx="10058400" cy="7533278"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_3" connectionId="6" xr16:uid="{FF5336E3-2BDB-41D1-B19E-626040BDB767}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="9">
-    <queryTableFields count="8">
+  <queryTableRefresh nextId="10">
+    <queryTableFields count="9">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
       <queryTableField id="2" name="Column2" tableColumnId="2"/>
       <queryTableField id="3" name="Column3" tableColumnId="3"/>
       <queryTableField id="4" name="Column4" tableColumnId="4"/>
       <queryTableField id="5" name="Column5" tableColumnId="5"/>
+      <queryTableField id="9" dataBound="0" tableColumnId="9"/>
       <queryTableField id="6" name="Column6" tableColumnId="6"/>
       <queryTableField id="7" name="Column7" tableColumnId="7"/>
       <queryTableField id="8" name="Column8" tableColumnId="8"/>
@@ -525,13 +936,14 @@
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_2" connectionId="4" xr16:uid="{7E5DF439-070E-4227-879C-0D33B8B8CC5D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="9">
-    <queryTableFields count="8">
+  <queryTableRefresh nextId="10">
+    <queryTableFields count="9">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
       <queryTableField id="2" name="Column2" tableColumnId="2"/>
       <queryTableField id="3" name="Column3" tableColumnId="3"/>
       <queryTableField id="4" name="Column4" tableColumnId="4"/>
       <queryTableField id="5" name="Column5" tableColumnId="5"/>
+      <queryTableField id="9" dataBound="0" tableColumnId="10"/>
       <queryTableField id="6" name="Column6" tableColumnId="6"/>
       <queryTableField id="7" name="Column7" tableColumnId="7"/>
       <queryTableField id="8" name="Column8" tableColumnId="8"/>
@@ -542,13 +954,14 @@
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="2" xr16:uid="{E8D43482-B6A0-4946-AD69-8EB6E137672F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="9">
-    <queryTableFields count="8">
+  <queryTableRefresh nextId="10">
+    <queryTableFields count="9">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
       <queryTableField id="2" name="Column2" tableColumnId="2"/>
       <queryTableField id="3" name="Column3" tableColumnId="3"/>
       <queryTableField id="4" name="Column4" tableColumnId="4"/>
       <queryTableField id="5" name="Column5" tableColumnId="5"/>
+      <queryTableField id="9" dataBound="0" tableColumnId="9"/>
       <queryTableField id="6" name="Column6" tableColumnId="6"/>
       <queryTableField id="7" name="Column7" tableColumnId="7"/>
       <queryTableField id="8" name="Column8" tableColumnId="8"/>
@@ -558,48 +971,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{79CF55FB-AC27-4977-80E3-AE31B1F9E902}" name="_7LevelSpecs__2" displayName="_7LevelSpecs__2" ref="A1:H23" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H23" xr:uid="{D117E7CA-7CCC-4FB2-A2F2-163E869A491D}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{2476D6BD-0915-4B24-9D82-5E9231E22D77}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{4CF90BC9-B4C3-41D5-8C88-A06417FFDF7B}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{8F806AAB-133E-4A82-9454-8E131DBFE1D8}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{C4172888-B421-400A-8DEC-390EAFCCD26A}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{F5884201-E201-474B-9A76-DEF5F634EBFC}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{D0DBC85D-0F55-4418-AB06-428040909B70}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{B3B89092-0BC3-4AAF-B496-453B56B7A2BB}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{53B00F5E-622A-4D47-B924-506153FED61A}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{79CF55FB-AC27-4977-80E3-AE31B1F9E902}" name="_7LevelSpecs__2" displayName="_7LevelSpecs__2" ref="A1:I23" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I23" xr:uid="{D117E7CA-7CCC-4FB2-A2F2-163E869A491D}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{2476D6BD-0915-4B24-9D82-5E9231E22D77}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{4CF90BC9-B4C3-41D5-8C88-A06417FFDF7B}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{8F806AAB-133E-4A82-9454-8E131DBFE1D8}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{C4172888-B421-400A-8DEC-390EAFCCD26A}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{F5884201-E201-474B-9A76-DEF5F634EBFC}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{352A67C9-4FA8-430F-AD46-FD2D93586B0D}" uniqueName="9" name="Column52" queryTableFieldId="9" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{D0DBC85D-0F55-4418-AB06-428040909B70}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{B3B89092-0BC3-4AAF-B496-453B56B7A2BB}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{53B00F5E-622A-4D47-B924-506153FED61A}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{70CCF9B6-75B8-4DD9-B0FC-957FF71188BF}" name="_5LevelSpecs__2" displayName="_5LevelSpecs__2" ref="A1:H14" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H14" xr:uid="{9B50E007-8865-4341-9D62-869EE222E5EA}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5CF240E7-3A14-4E8A-9295-61A936507CEA}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{841727CD-2B9D-4C52-9AB6-B385465C759C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{625C9E86-0464-44A7-A529-F84EDEB3FA24}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{D2708508-5005-4E32-A10E-28A49DC653C4}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{73595F5F-FD93-4E26-8EBB-EDB1FFE8DA89}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{B5E51F02-5F9F-430D-8A72-4A6B769554A4}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{AA219D7B-39F5-4B9E-A10D-B0F06F42CBF6}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{D3049359-DD44-4E1C-B330-561BFDF0EFA6}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{70CCF9B6-75B8-4DD9-B0FC-957FF71188BF}" name="_5LevelSpecs__2" displayName="_5LevelSpecs__2" ref="A1:I14" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I14" xr:uid="{9B50E007-8865-4341-9D62-869EE222E5EA}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{5CF240E7-3A14-4E8A-9295-61A936507CEA}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{841727CD-2B9D-4C52-9AB6-B385465C759C}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{625C9E86-0464-44A7-A529-F84EDEB3FA24}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{D2708508-5005-4E32-A10E-28A49DC653C4}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{73595F5F-FD93-4E26-8EBB-EDB1FFE8DA89}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{888291B9-3CEA-4FE1-AC99-64DE91049843}" uniqueName="10" name="Column52" queryTableFieldId="9" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{B5E51F02-5F9F-430D-8A72-4A6B769554A4}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{AA219D7B-39F5-4B9E-A10D-B0F06F42CBF6}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{D3049359-DD44-4E1C-B330-561BFDF0EFA6}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70FF07AA-009B-4D8A-AA9B-D3A29CEC053D}" name="_3LevelSpecs__2" displayName="_3LevelSpecs__2" ref="A1:H7" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H7" xr:uid="{00C95859-DBC4-405B-A211-3A30F6936B0F}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{6C1065F4-6D44-46AF-B825-56E8FF7276F9}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{275DEE58-63B2-41C1-B58E-7A47A8A04610}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{63AA929F-6DFE-4D4D-889F-3859B3FFD663}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{0E7477EB-840A-4393-A118-7CBD1B5236B0}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{D326AB46-9967-4210-B41B-44C6A83F401D}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70FF07AA-009B-4D8A-AA9B-D3A29CEC053D}" name="_3LevelSpecs__2" displayName="_3LevelSpecs__2" ref="A1:I7" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I7" xr:uid="{00C95859-DBC4-405B-A211-3A30F6936B0F}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{6C1065F4-6D44-46AF-B825-56E8FF7276F9}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{275DEE58-63B2-41C1-B58E-7A47A8A04610}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{63AA929F-6DFE-4D4D-889F-3859B3FFD663}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{0E7477EB-840A-4393-A118-7CBD1B5236B0}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{D326AB46-9967-4210-B41B-44C6A83F401D}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{887962EE-3C1A-4D6D-ACE1-2136198EA2B4}" uniqueName="9" name="Column52" queryTableFieldId="9" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{000D7740-7C37-4BB2-99C2-BE83673E63CD}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{F561C63A-303F-4F3F-BF4C-742F3F2D2ECC}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{FEF2FC01-EEFF-41F6-BA12-09C0DDAF7003}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="0"/>
@@ -905,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7ACD215-AF42-4B41-941C-7E6ED12B4E69}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -916,14 +1332,16 @@
     <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.20703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.89453125" customWidth="1"/>
     <col min="5" max="5" width="15.20703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.20703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.20703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83984375" customWidth="1"/>
+    <col min="6" max="6" width="15.20703125" customWidth="1"/>
+    <col min="7" max="7" width="19.20703125" customWidth="1"/>
+    <col min="8" max="8" width="20.7890625" customWidth="1"/>
+    <col min="9" max="9" width="22.26171875" customWidth="1"/>
+    <col min="10" max="10" width="8.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -940,21 +1358,24 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -966,16 +1387,19 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -983,25 +1407,31 @@
         <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>35</v>
+        <v>59</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3982050647.5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1.3272488609979E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1009,25 +1439,31 @@
         <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>54</v>
+        <v>69</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3999321567.6999998</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1.2733105671904001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4">
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1035,77 +1471,86 @@
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>70</v>
+      </c>
+      <c r="F5" s="2">
+        <v>4016150785.5999999</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1.3272488609979E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>36</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1113,51 +1558,57 @@
         <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>71</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4102645765.1599998</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1.2999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>35</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1165,51 +1616,57 @@
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4106913074.98</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" s="2">
-        <v>2.2603911202810998E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="I10" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>36</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1217,33 +1674,36 @@
         <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
+      </c>
+      <c r="F12" s="2">
+        <v>4114887145.5100002</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" s="2">
-        <v>2.1093738732015001E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>16</v>
@@ -1251,51 +1711,57 @@
       <c r="E13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>16</v>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>35</v>
+        <v>74</v>
+      </c>
+      <c r="F14" s="2">
+        <v>3982050647.5</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="2">
-        <v>1.3272488609979E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>16</v>
@@ -1303,51 +1769,57 @@
       <c r="E15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>16</v>
+      <c r="F15" s="2">
+        <v>0</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>54</v>
+        <v>89</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3999321567.6999998</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="2">
-        <v>1.2733105671904001E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>16</v>
@@ -1355,51 +1827,57 @@
       <c r="E17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>16</v>
+      <c r="F17" s="2">
+        <v>0</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>25</v>
+        <v>90</v>
+      </c>
+      <c r="F18" s="2">
+        <v>4016150785.5999999</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="2">
-        <v>1.3090202209187999E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>16</v>
@@ -1407,51 +1885,57 @@
       <c r="E19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>16</v>
+      <c r="F19" s="2">
+        <v>0</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>63</v>
+        <v>91</v>
+      </c>
+      <c r="F20" s="2">
+        <v>4106913074.98</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1.8117050564913999E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>16</v>
@@ -1459,51 +1943,57 @@
       <c r="E21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>16</v>
+      <c r="F21" s="2">
+        <v>0</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>42</v>
+        <v>92</v>
+      </c>
+      <c r="F22" s="2">
+        <v>4102645765.1599998</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H22" s="2">
-        <v>1.2821455999707E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3">
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>16</v>
@@ -1511,114 +2001,716 @@
       <c r="E23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>16</v>
+      <c r="F23" s="2">
+        <v>0</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="6" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="4">
         <v>0</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="F26" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="4">
         <v>1</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="F27" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="4">
         <v>2</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="F28" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="4">
         <v>3</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5">
         <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="10">
+        <v>1</v>
+      </c>
+      <c r="B33" s="11">
+        <v>0</v>
+      </c>
+      <c r="C33" s="11">
+        <v>0.99882040542544004</v>
+      </c>
+      <c r="D33" s="11">
+        <v>30700</v>
+      </c>
+      <c r="E33" s="11">
+        <v>979469667.06954002</v>
+      </c>
+      <c r="F33" s="11">
+        <v>3980750647.5</v>
+      </c>
+      <c r="G33" s="11">
+        <v>3983350647.5</v>
+      </c>
+      <c r="H33" s="11">
+        <v>1.327249E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="12">
+        <v>2</v>
+      </c>
+      <c r="B34" s="9">
+        <v>0</v>
+      </c>
+      <c r="C34" s="9">
+        <v>0.99884771116372995</v>
+      </c>
+      <c r="D34" s="9">
+        <v>31400</v>
+      </c>
+      <c r="E34" s="9">
+        <v>1020960662.306</v>
+      </c>
+      <c r="F34" s="9">
+        <v>3998021567.6999998</v>
+      </c>
+      <c r="G34" s="9">
+        <v>4000621567.6999998</v>
+      </c>
+      <c r="H34" s="9">
+        <v>1.2733110000000001E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="10">
+        <v>3</v>
+      </c>
+      <c r="B35" s="11">
+        <v>0</v>
+      </c>
+      <c r="C35" s="11">
+        <v>0.99881959919827001</v>
+      </c>
+      <c r="D35" s="11">
+        <v>30700</v>
+      </c>
+      <c r="E35" s="11">
+        <v>979469667.06954002</v>
+      </c>
+      <c r="F35" s="11">
+        <v>4014850785.5999999</v>
+      </c>
+      <c r="G35" s="11">
+        <v>4017450785.5999999</v>
+      </c>
+      <c r="H35" s="11">
+        <v>1.327249E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="12">
+        <v>4</v>
+      </c>
+      <c r="B36" s="9">
+        <v>2</v>
+      </c>
+      <c r="C36" s="9">
+        <v>0</v>
+      </c>
+      <c r="D36" s="9">
+        <v>0</v>
+      </c>
+      <c r="E36" s="9">
+        <v>0</v>
+      </c>
+      <c r="F36" s="9">
+        <v>8044335950</v>
+      </c>
+      <c r="G36" s="9">
+        <v>8044335950</v>
+      </c>
+      <c r="H36" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="10">
+        <v>5</v>
+      </c>
+      <c r="B37" s="11">
+        <v>2</v>
+      </c>
+      <c r="C37" s="11">
+        <v>0</v>
+      </c>
+      <c r="D37" s="11">
+        <v>0</v>
+      </c>
+      <c r="E37" s="11">
+        <v>0</v>
+      </c>
+      <c r="F37" s="11">
+        <v>8031164238</v>
+      </c>
+      <c r="G37" s="11">
+        <v>8031164238</v>
+      </c>
+      <c r="H37" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="12">
+        <v>6</v>
+      </c>
+      <c r="B38" s="9">
+        <v>0</v>
+      </c>
+      <c r="C38" s="9">
+        <v>0.99883515374099996</v>
+      </c>
+      <c r="D38" s="9">
+        <v>31100</v>
+      </c>
+      <c r="E38" s="9">
+        <v>1000000000</v>
+      </c>
+      <c r="F38" s="9">
+        <v>4101345765.1599998</v>
+      </c>
+      <c r="G38" s="9">
+        <v>4103945765.1599998</v>
+      </c>
+      <c r="H38" s="9">
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="10">
+        <v>7</v>
+      </c>
+      <c r="B39" s="11">
+        <v>2</v>
+      </c>
+      <c r="C39" s="11">
+        <v>0</v>
+      </c>
+      <c r="D39" s="11">
+        <v>0</v>
+      </c>
+      <c r="E39" s="11">
+        <v>0</v>
+      </c>
+      <c r="F39" s="11">
+        <v>8044335950</v>
+      </c>
+      <c r="G39" s="11">
+        <v>8044335950</v>
+      </c>
+      <c r="H39" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="12">
+        <v>8</v>
+      </c>
+      <c r="B40" s="9">
+        <v>0</v>
+      </c>
+      <c r="C40" s="9">
+        <v>0.99839081139348995</v>
+      </c>
+      <c r="D40" s="9">
+        <v>23100</v>
+      </c>
+      <c r="E40" s="9">
+        <v>575121707.18415999</v>
+      </c>
+      <c r="F40" s="9">
+        <v>4105613074.98</v>
+      </c>
+      <c r="G40" s="9">
+        <v>4108213074.98</v>
+      </c>
+      <c r="H40" s="9">
+        <v>2.260391E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="10">
+        <v>9</v>
+      </c>
+      <c r="B41" s="11">
+        <v>2</v>
+      </c>
+      <c r="C41" s="11">
+        <v>0</v>
+      </c>
+      <c r="D41" s="11">
+        <v>0</v>
+      </c>
+      <c r="E41" s="11">
+        <v>0</v>
+      </c>
+      <c r="F41" s="11">
+        <v>8031164238</v>
+      </c>
+      <c r="G41" s="11">
+        <v>8031164238</v>
+      </c>
+      <c r="H41" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="12">
+        <v>10</v>
+      </c>
+      <c r="B42" s="9">
+        <v>0</v>
+      </c>
+      <c r="C42" s="9">
+        <v>0.99846491248735003</v>
+      </c>
+      <c r="D42" s="9">
+        <v>24000</v>
+      </c>
+      <c r="E42" s="9">
+        <v>616296625.51329005</v>
+      </c>
+      <c r="F42" s="9">
+        <v>4113587145.5100002</v>
+      </c>
+      <c r="G42" s="9">
+        <v>4116187145.5100002</v>
+      </c>
+      <c r="H42" s="9">
+        <v>2.1093739999999998E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="10">
+        <v>11</v>
+      </c>
+      <c r="B43" s="11">
+        <v>3</v>
+      </c>
+      <c r="C43" s="11">
+        <v>0</v>
+      </c>
+      <c r="D43" s="11">
+        <v>0</v>
+      </c>
+      <c r="E43" s="11">
+        <v>0</v>
+      </c>
+      <c r="F43" s="11">
+        <v>0</v>
+      </c>
+      <c r="G43" s="11">
+        <v>0</v>
+      </c>
+      <c r="H43" s="13">
+        <v>3.6999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="12">
+        <v>12</v>
+      </c>
+      <c r="B44" s="9">
+        <v>1</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0.99882054956258004</v>
+      </c>
+      <c r="D44" s="9">
+        <v>30700</v>
+      </c>
+      <c r="E44" s="9">
+        <v>979469667.06954002</v>
+      </c>
+      <c r="F44" s="9">
+        <v>3980750647.5</v>
+      </c>
+      <c r="G44" s="9">
+        <v>3983350647.5</v>
+      </c>
+      <c r="H44" s="9">
+        <v>1.327249E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="10">
+        <v>13</v>
+      </c>
+      <c r="B45" s="11">
+        <v>3</v>
+      </c>
+      <c r="C45" s="11">
+        <v>0</v>
+      </c>
+      <c r="D45" s="11">
+        <v>0</v>
+      </c>
+      <c r="E45" s="11">
+        <v>0</v>
+      </c>
+      <c r="F45" s="11">
+        <v>0</v>
+      </c>
+      <c r="G45" s="11">
+        <v>0</v>
+      </c>
+      <c r="H45" s="13">
+        <v>3.6999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="12">
+        <v>14</v>
+      </c>
+      <c r="B46" s="9">
+        <v>1</v>
+      </c>
+      <c r="C46" s="9">
+        <v>0.99884800011184005</v>
+      </c>
+      <c r="D46" s="9">
+        <v>31400</v>
+      </c>
+      <c r="E46" s="9">
+        <v>1020960662.306</v>
+      </c>
+      <c r="F46" s="9">
+        <v>3998021567.6999998</v>
+      </c>
+      <c r="G46" s="9">
+        <v>4000621567.6999998</v>
+      </c>
+      <c r="H46" s="9">
+        <v>1.2733110000000001E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="10">
+        <v>15</v>
+      </c>
+      <c r="B47" s="11">
+        <v>3</v>
+      </c>
+      <c r="C47" s="11">
+        <v>0</v>
+      </c>
+      <c r="D47" s="11">
+        <v>0</v>
+      </c>
+      <c r="E47" s="11">
+        <v>0</v>
+      </c>
+      <c r="F47" s="11">
+        <v>0</v>
+      </c>
+      <c r="G47" s="11">
+        <v>0</v>
+      </c>
+      <c r="H47" s="13">
+        <v>3.6999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="12">
+        <v>16</v>
+      </c>
+      <c r="B48" s="9">
+        <v>1</v>
+      </c>
+      <c r="C48" s="9">
+        <v>0.99882829332992995</v>
+      </c>
+      <c r="D48" s="9">
+        <v>30900</v>
+      </c>
+      <c r="E48" s="9">
+        <v>993109181.37497997</v>
+      </c>
+      <c r="F48" s="9">
+        <v>4014850785.5999999</v>
+      </c>
+      <c r="G48" s="9">
+        <v>4017450785.5999999</v>
+      </c>
+      <c r="H48" s="9">
+        <v>1.3090199999999999E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="10">
+        <v>17</v>
+      </c>
+      <c r="B49" s="11">
+        <v>3</v>
+      </c>
+      <c r="C49" s="11">
+        <v>0</v>
+      </c>
+      <c r="D49" s="11">
+        <v>0</v>
+      </c>
+      <c r="E49" s="11">
+        <v>0</v>
+      </c>
+      <c r="F49" s="11">
+        <v>0</v>
+      </c>
+      <c r="G49" s="11">
+        <v>0</v>
+      </c>
+      <c r="H49" s="13">
+        <v>3.6999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="12">
+        <v>18</v>
+      </c>
+      <c r="B50" s="9">
+        <v>1</v>
+      </c>
+      <c r="C50" s="9">
+        <v>0.99858763254548</v>
+      </c>
+      <c r="D50" s="9">
+        <v>26000</v>
+      </c>
+      <c r="E50" s="9">
+        <v>717556091.89368999</v>
+      </c>
+      <c r="F50" s="9">
+        <v>4105613074.98</v>
+      </c>
+      <c r="G50" s="9">
+        <v>4108213074.98</v>
+      </c>
+      <c r="H50" s="9">
+        <v>1.811705E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="10">
+        <v>19</v>
+      </c>
+      <c r="B51" s="11">
+        <v>3</v>
+      </c>
+      <c r="C51" s="11">
+        <v>0</v>
+      </c>
+      <c r="D51" s="11">
+        <v>0</v>
+      </c>
+      <c r="E51" s="11">
+        <v>0</v>
+      </c>
+      <c r="F51" s="11">
+        <v>0</v>
+      </c>
+      <c r="G51" s="11">
+        <v>0</v>
+      </c>
+      <c r="H51" s="13">
+        <v>3.6999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="12">
+        <v>20</v>
+      </c>
+      <c r="B52" s="9">
+        <v>1</v>
+      </c>
+      <c r="C52" s="9">
+        <v>0.99884519595553001</v>
+      </c>
+      <c r="D52" s="9">
+        <v>31300</v>
+      </c>
+      <c r="E52" s="9">
+        <v>1013925407.5588</v>
+      </c>
+      <c r="F52" s="9">
+        <v>4101345765.1599998</v>
+      </c>
+      <c r="G52" s="9">
+        <v>4103945765.1599998</v>
+      </c>
+      <c r="H52" s="9">
+        <v>1.2821460000000001E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="10">
+        <v>21</v>
+      </c>
+      <c r="B53" s="11">
+        <v>3</v>
+      </c>
+      <c r="C53" s="11">
+        <v>0</v>
+      </c>
+      <c r="D53" s="11">
+        <v>0</v>
+      </c>
+      <c r="E53" s="11">
+        <v>0</v>
+      </c>
+      <c r="F53" s="11">
+        <v>0</v>
+      </c>
+      <c r="G53" s="11">
+        <v>0</v>
+      </c>
+      <c r="H53" s="13">
+        <v>3.6999999999999998E-5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01FA352F-6AFF-43CD-9A43-30E5B46DF47C}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1626,14 +2718,16 @@
     <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.20703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.20703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.20703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.20703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83984375" customWidth="1"/>
+    <col min="4" max="4" width="17.5234375" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="15.3125" customWidth="1"/>
+    <col min="7" max="7" width="19.83984375" customWidth="1"/>
+    <col min="8" max="8" width="20.578125" customWidth="1"/>
+    <col min="9" max="9" width="24.26171875" customWidth="1"/>
+    <col min="10" max="10" width="8.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1650,21 +2744,24 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -1676,16 +2773,22 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="K2" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1693,25 +2796,31 @@
         <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>25</v>
+        <v>59</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4016150785.5999999</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1.3181030298264999E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3">
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1719,51 +2828,57 @@
         <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>69</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3982050647.5</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1.3090202209187999E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1771,25 +2886,28 @@
         <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>42</v>
+        <v>70</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4102645765.1599998</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1.2999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1797,33 +2915,36 @@
         <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>20</v>
+        <v>71</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4111019937.1100001</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1.3090202209187999E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>16</v>
@@ -1831,51 +2952,57 @@
       <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>16</v>
+      <c r="F8" s="2">
+        <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>20</v>
+        <v>72</v>
+      </c>
+      <c r="F9" s="2">
+        <v>4111019937.1100001</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1.3090202209187999E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>16</v>
@@ -1883,51 +3010,57 @@
       <c r="E10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>16</v>
+      <c r="F10" s="2">
+        <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>35</v>
+        <v>73</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3982050647.5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="2">
-        <v>1.3090202209187999E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>16</v>
@@ -1935,51 +3068,57 @@
       <c r="E12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>16</v>
+      <c r="F12" s="2">
+        <v>0</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>25</v>
+        <v>74</v>
+      </c>
+      <c r="F13" s="2">
+        <v>4016150785.5999999</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="2">
-        <v>1.3090202209187999E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>16</v>
@@ -1987,114 +3126,482 @@
       <c r="E14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>16</v>
+      <c r="F14" s="2">
+        <v>0</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="6" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="4">
         <v>0</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="F18" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="4">
         <v>1</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="F19" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="4">
         <v>2</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="F20" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="4">
         <v>3</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5">
         <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="10">
+        <v>1</v>
+      </c>
+      <c r="B25" s="11">
+        <v>0</v>
+      </c>
+      <c r="C25" s="11">
+        <v>0.99882773258697999</v>
+      </c>
+      <c r="D25" s="11">
+        <v>30800</v>
+      </c>
+      <c r="E25" s="11">
+        <v>986265846.13127995</v>
+      </c>
+      <c r="F25" s="11">
+        <v>4014850785.5999999</v>
+      </c>
+      <c r="G25" s="11">
+        <v>4017450785.5999999</v>
+      </c>
+      <c r="H25" s="11">
+        <v>1.3181029999999999E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="12">
+        <v>2</v>
+      </c>
+      <c r="B26" s="9">
+        <v>0</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0.99882971046946001</v>
+      </c>
+      <c r="D26" s="9">
+        <v>30900</v>
+      </c>
+      <c r="E26" s="9">
+        <v>993109181.37497997</v>
+      </c>
+      <c r="F26" s="9">
+        <v>3980750647.5</v>
+      </c>
+      <c r="G26" s="9">
+        <v>3983350647.5</v>
+      </c>
+      <c r="H26" s="9">
+        <v>1.3090199999999999E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="10">
+        <v>3</v>
+      </c>
+      <c r="B27" s="11">
+        <v>2</v>
+      </c>
+      <c r="C27" s="11">
+        <v>0</v>
+      </c>
+      <c r="D27" s="11">
+        <v>0</v>
+      </c>
+      <c r="E27" s="11">
+        <v>0</v>
+      </c>
+      <c r="F27" s="11">
+        <v>8027867256</v>
+      </c>
+      <c r="G27" s="11">
+        <v>8027867256</v>
+      </c>
+      <c r="H27" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="12">
+        <v>4</v>
+      </c>
+      <c r="B28" s="9">
+        <v>0</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0.99883564341251996</v>
+      </c>
+      <c r="D28" s="9">
+        <v>31100</v>
+      </c>
+      <c r="E28" s="9">
+        <v>1000000000</v>
+      </c>
+      <c r="F28" s="9">
+        <v>4101345765.1599998</v>
+      </c>
+      <c r="G28" s="9">
+        <v>4103945765.1599998</v>
+      </c>
+      <c r="H28" s="9">
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="10">
+        <v>5</v>
+      </c>
+      <c r="B29" s="11">
+        <v>0</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0.99883229496339998</v>
+      </c>
+      <c r="D29" s="11">
+        <v>30900</v>
+      </c>
+      <c r="E29" s="11">
+        <v>993109181.37497997</v>
+      </c>
+      <c r="F29" s="11">
+        <v>4109719937.1100001</v>
+      </c>
+      <c r="G29" s="11">
+        <v>4112319937.1100001</v>
+      </c>
+      <c r="H29" s="11">
+        <v>1.3090199999999999E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="12">
+        <v>6</v>
+      </c>
+      <c r="B30" s="9">
+        <v>3</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0</v>
+      </c>
+      <c r="D30" s="9">
+        <v>0</v>
+      </c>
+      <c r="E30" s="9">
+        <v>0</v>
+      </c>
+      <c r="F30" s="9">
+        <v>0</v>
+      </c>
+      <c r="G30" s="9">
+        <v>0</v>
+      </c>
+      <c r="H30" s="15">
+        <v>3.6999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="10">
+        <v>7</v>
+      </c>
+      <c r="B31" s="11">
+        <v>1</v>
+      </c>
+      <c r="C31" s="11">
+        <v>0.99883239561794002</v>
+      </c>
+      <c r="D31" s="11">
+        <v>30900</v>
+      </c>
+      <c r="E31" s="11">
+        <v>993109181.37497997</v>
+      </c>
+      <c r="F31" s="11">
+        <v>4109719937.1100001</v>
+      </c>
+      <c r="G31" s="11">
+        <v>4112319937.1100001</v>
+      </c>
+      <c r="H31" s="11">
+        <v>1.3090199999999999E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="12">
+        <v>8</v>
+      </c>
+      <c r="B32" s="9">
+        <v>3</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0</v>
+      </c>
+      <c r="E32" s="9">
+        <v>0</v>
+      </c>
+      <c r="F32" s="9">
+        <v>0</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0</v>
+      </c>
+      <c r="H32" s="15">
+        <v>3.6999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="10">
+        <v>9</v>
+      </c>
+      <c r="B33" s="11">
+        <v>1</v>
+      </c>
+      <c r="C33" s="11">
+        <v>0.99882948368628</v>
+      </c>
+      <c r="D33" s="11">
+        <v>30900</v>
+      </c>
+      <c r="E33" s="11">
+        <v>993109181.37497997</v>
+      </c>
+      <c r="F33" s="11">
+        <v>3980750647.5</v>
+      </c>
+      <c r="G33" s="11">
+        <v>3983350647.5</v>
+      </c>
+      <c r="H33" s="11">
+        <v>1.3090199999999999E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="12">
+        <v>10</v>
+      </c>
+      <c r="B34" s="9">
+        <v>3</v>
+      </c>
+      <c r="C34" s="9">
+        <v>0</v>
+      </c>
+      <c r="D34" s="9">
+        <v>0</v>
+      </c>
+      <c r="E34" s="9">
+        <v>0</v>
+      </c>
+      <c r="F34" s="9">
+        <v>0</v>
+      </c>
+      <c r="G34" s="9">
+        <v>0</v>
+      </c>
+      <c r="H34" s="15">
+        <v>3.6999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="10">
+        <v>11</v>
+      </c>
+      <c r="B35" s="11">
+        <v>1</v>
+      </c>
+      <c r="C35" s="11">
+        <v>0.99882854571752</v>
+      </c>
+      <c r="D35" s="11">
+        <v>30900</v>
+      </c>
+      <c r="E35" s="11">
+        <v>993109181.37497997</v>
+      </c>
+      <c r="F35" s="11">
+        <v>4014850785.5999999</v>
+      </c>
+      <c r="G35" s="11">
+        <v>4017450785.5999999</v>
+      </c>
+      <c r="H35" s="11">
+        <v>1.3090199999999999E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="12">
+        <v>12</v>
+      </c>
+      <c r="B36" s="9">
+        <v>3</v>
+      </c>
+      <c r="C36" s="9">
+        <v>0</v>
+      </c>
+      <c r="D36" s="9">
+        <v>0</v>
+      </c>
+      <c r="E36" s="9">
+        <v>0</v>
+      </c>
+      <c r="F36" s="9">
+        <v>0</v>
+      </c>
+      <c r="G36" s="9">
+        <v>0</v>
+      </c>
+      <c r="H36" s="15">
+        <v>3.6999999999999998E-5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0277561-7EE0-4C2E-94B3-85E4C94A3B2A}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2102,14 +3609,16 @@
     <col min="1" max="1" width="10.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.20703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.20703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.20703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.20703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83984375" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="20.578125" customWidth="1"/>
+    <col min="6" max="6" width="15.20703125" customWidth="1"/>
+    <col min="7" max="7" width="17.41796875" customWidth="1"/>
+    <col min="8" max="8" width="17.83984375" customWidth="1"/>
+    <col min="9" max="9" width="20.89453125" customWidth="1"/>
+    <col min="10" max="10" width="8.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2126,21 +3635,24 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -2152,16 +3664,19 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2172,22 +3687,28 @@
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>59</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4111019937.1100001</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1.2821455999707E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2195,33 +3716,39 @@
         <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>69</v>
+      </c>
+      <c r="F4" s="2">
+        <v>4016150785.5999999</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1.3181030298264999E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4">
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
@@ -2229,51 +3756,57 @@
       <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>16</v>
+      <c r="F5" s="2">
+        <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>16</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
+        <v>70</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4111019937.1100001</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1.2821455999707E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>16</v>
@@ -2281,104 +3814,290 @@
       <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="6" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="4">
         <v>0</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="F11" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="4">
         <v>1</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="F12" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="4">
         <v>2</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="F13" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="4">
         <v>3</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5">
         <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="10">
+        <v>1</v>
+      </c>
+      <c r="B19" s="11">
+        <v>0</v>
+      </c>
+      <c r="C19" s="11">
+        <v>0.99884260753762999</v>
+      </c>
+      <c r="D19" s="11">
+        <v>31300</v>
+      </c>
+      <c r="E19" s="11">
+        <v>1013925407.5588</v>
+      </c>
+      <c r="F19" s="11">
+        <v>4109719937.1100001</v>
+      </c>
+      <c r="G19" s="11">
+        <v>4112319937.1100001</v>
+      </c>
+      <c r="H19" s="11">
+        <v>1.2821460000000001E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="12">
+        <v>2</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.99882794762124005</v>
+      </c>
+      <c r="D20" s="9">
+        <v>30800</v>
+      </c>
+      <c r="E20" s="9">
+        <v>986265846.13127995</v>
+      </c>
+      <c r="F20" s="9">
+        <v>4014850785.5999999</v>
+      </c>
+      <c r="G20" s="9">
+        <v>4017450785.5999999</v>
+      </c>
+      <c r="H20" s="9">
+        <v>1.3181029999999999E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="10">
+        <v>3</v>
+      </c>
+      <c r="B21" s="11">
+        <v>3</v>
+      </c>
+      <c r="C21" s="11">
+        <v>0</v>
+      </c>
+      <c r="D21" s="11">
+        <v>0</v>
+      </c>
+      <c r="E21" s="11">
+        <v>0</v>
+      </c>
+      <c r="F21" s="11">
+        <v>0</v>
+      </c>
+      <c r="G21" s="11">
+        <v>0</v>
+      </c>
+      <c r="H21" s="13">
+        <v>3.6999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="12">
+        <v>4</v>
+      </c>
+      <c r="B22" s="9">
+        <v>1</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.99884293155388004</v>
+      </c>
+      <c r="D22" s="9">
+        <v>31300</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1013925407.5588</v>
+      </c>
+      <c r="F22" s="9">
+        <v>4109719937.1100001</v>
+      </c>
+      <c r="G22" s="9">
+        <v>4112319937.1100001</v>
+      </c>
+      <c r="H22" s="9">
+        <v>1.2821460000000001E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="10">
+        <v>5</v>
+      </c>
+      <c r="B23" s="11">
+        <v>3</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0</v>
+      </c>
+      <c r="D23" s="11">
+        <v>0</v>
+      </c>
+      <c r="E23" s="11">
+        <v>0</v>
+      </c>
+      <c r="F23" s="11">
+        <v>0</v>
+      </c>
+      <c r="G23" s="11">
+        <v>0</v>
+      </c>
+      <c r="H23" s="13">
+        <v>3.6999999999999998E-5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>